<commit_message>
ICSP + Serigraphie done
</commit_message>
<xml_diff>
--- a/Altium/Project Outputs for ThumbsUp/BOM/Bill of Materials-ThumbsUp.xlsx
+++ b/Altium/Project Outputs for ThumbsUp/BOM/Bill of Materials-ThumbsUp.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17145" windowHeight="12405"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23580" windowHeight="12405"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-ThumbsUp" sheetId="1" r:id="rId1"/>
@@ -90,13 +90,13 @@
     <t>J1</t>
   </si>
   <si>
-    <t>AMP - TE CONNECTIVITY</t>
-  </si>
-  <si>
-    <t>826629-6</t>
-  </si>
-  <si>
-    <t>3418327</t>
+    <t>MOLEX</t>
+  </si>
+  <si>
+    <t>22-27-2061</t>
+  </si>
+  <si>
+    <t>9731172</t>
   </si>
   <si>
     <t>L2</t>

</xml_diff>